<commit_message>
waste calc - excel main data
</commit_message>
<xml_diff>
--- a/data_calc/kalkulacka_data.XLSX
+++ b/data_calc/kalkulacka_data.XLSX
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\x_other\eta_code_work\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6A3DD5C-C055-4F20-9E32-FD529ABAF38B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="10610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="List2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="70">
   <si>
     <t>Kraj</t>
   </si>
@@ -143,13 +138,121 @@
   </si>
   <si>
     <t>Data pro kalkulačku</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>nakladyNaOhKc</t>
+  </si>
+  <si>
+    <t>nakladyZOhKc</t>
+  </si>
+  <si>
+    <t>nakladyTridenySberTun</t>
+  </si>
+  <si>
+    <t>nakladyTridenySberKc</t>
+  </si>
+  <si>
+    <t>nakladySkoTun</t>
+  </si>
+  <si>
+    <t>nakladySkoKc</t>
+  </si>
+  <si>
+    <t>produkceOdpadCelkova</t>
+  </si>
+  <si>
+    <t>produkceOdpadO</t>
+  </si>
+  <si>
+    <t>produkceOdpadN</t>
+  </si>
+  <si>
+    <t>produkceKomunal</t>
+  </si>
+  <si>
+    <t>produkceSko</t>
+  </si>
+  <si>
+    <t>produkcePlast</t>
+  </si>
+  <si>
+    <t>produkcePapir</t>
+  </si>
+  <si>
+    <t>produkceSklo</t>
+  </si>
+  <si>
+    <t>produkceKovy</t>
+  </si>
+  <si>
+    <t>produkceBro</t>
+  </si>
+  <si>
+    <t>regionCode</t>
+  </si>
+  <si>
+    <t>jm</t>
+  </si>
+  <si>
+    <t>kr</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>zl</t>
+  </si>
+  <si>
+    <t>vy</t>
+  </si>
+  <si>
+    <t>ol</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>us</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>li</t>
+  </si>
+  <si>
+    <t>pl</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>jc</t>
+  </si>
+  <si>
+    <t>cr</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,8 +270,25 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,8 +313,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -305,19 +437,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -351,17 +470,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -470,46 +578,29 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -517,24 +608,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -555,55 +641,59 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -876,771 +966,1230 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" customWidth="1"/>
+    <col min="10" max="10" width="8.54296875" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" customWidth="1"/>
+    <col min="12" max="12" width="6.26953125" customWidth="1"/>
+    <col min="13" max="13" width="19.7265625" customWidth="1"/>
+    <col min="14" max="14" width="11.54296875" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" customWidth="1"/>
+    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B1" s="30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:18" ht="69.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:19" ht="69.650000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="P3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="R3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="35" t="s">
+      <c r="S3" s="28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:19" s="31" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" s="34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14">
+      <c r="C5" s="11">
         <v>1184729</v>
       </c>
-      <c r="C4" s="13">
+      <c r="D5" s="10">
         <v>949</v>
       </c>
-      <c r="D4" s="13">
+      <c r="E5" s="10">
         <v>628</v>
       </c>
-      <c r="E4" s="14">
+      <c r="F5" s="11">
         <v>3293</v>
       </c>
-      <c r="F4" s="13">
+      <c r="G5" s="10">
         <v>109</v>
       </c>
-      <c r="G4" s="13">
+      <c r="H5" s="10">
         <v>2731</v>
       </c>
-      <c r="H4" s="13">
+      <c r="I5" s="10">
         <v>500</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J5" s="2">
         <v>4437</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K5" s="2">
         <v>4286</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L5" s="3">
         <v>151</v>
       </c>
-      <c r="L4" s="13">
+      <c r="M5" s="10">
         <v>512</v>
       </c>
-      <c r="M4" s="24">
+      <c r="N5" s="19">
         <v>251</v>
       </c>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="29"/>
-    </row>
-    <row r="5" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="22"/>
+    </row>
+    <row r="6" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16">
+      <c r="C6" s="13">
         <v>550688</v>
       </c>
-      <c r="C5" s="15">
+      <c r="D6" s="12">
         <v>969</v>
       </c>
-      <c r="D5" s="15">
+      <c r="E6" s="12">
         <v>521</v>
       </c>
-      <c r="E5" s="16">
+      <c r="F6" s="13">
         <v>4294</v>
       </c>
-      <c r="F5" s="15">
+      <c r="G6" s="12">
         <v>181</v>
       </c>
-      <c r="G5" s="15">
+      <c r="H6" s="12">
         <v>2385</v>
       </c>
-      <c r="H5" s="15">
+      <c r="I6" s="12">
         <v>447</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J6" s="4">
         <v>3045</v>
       </c>
-      <c r="J5" s="4">
+      <c r="K6" s="4">
         <v>2933</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L6" s="5">
         <v>112</v>
       </c>
-      <c r="L5" s="15">
+      <c r="M6" s="12">
         <v>553</v>
       </c>
-      <c r="M5" s="25">
+      <c r="N6" s="20">
         <v>259</v>
       </c>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-    </row>
-    <row r="6" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+    </row>
+    <row r="7" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16">
+      <c r="C7" s="13">
         <v>1204346</v>
       </c>
-      <c r="C6" s="15">
+      <c r="D7" s="12">
         <v>1016</v>
       </c>
-      <c r="D6" s="15">
+      <c r="E7" s="12">
         <v>569</v>
       </c>
-      <c r="E6" s="16">
+      <c r="F7" s="13">
         <v>3933</v>
       </c>
-      <c r="F6" s="15">
+      <c r="G7" s="12">
         <v>146</v>
       </c>
-      <c r="G6" s="15">
+      <c r="H7" s="12">
         <v>2474</v>
       </c>
-      <c r="H6" s="15">
+      <c r="I7" s="12">
         <v>464</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J7" s="4">
         <v>3844</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K7" s="4">
         <v>3528</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L7" s="5">
         <v>316</v>
       </c>
-      <c r="L6" s="15">
+      <c r="M7" s="12">
         <v>542</v>
       </c>
-      <c r="M6" s="25">
+      <c r="N7" s="20">
         <v>245</v>
       </c>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-    </row>
-    <row r="7" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+    </row>
+    <row r="8" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16">
+      <c r="C8" s="13">
         <v>582860</v>
       </c>
-      <c r="C7" s="15">
+      <c r="D8" s="12">
         <v>1028</v>
       </c>
-      <c r="D7" s="15">
+      <c r="E8" s="12">
         <v>536</v>
       </c>
-      <c r="E7" s="16">
+      <c r="F8" s="13">
         <v>3970</v>
       </c>
-      <c r="F7" s="15">
+      <c r="G8" s="12">
         <v>137</v>
       </c>
-      <c r="G7" s="15">
+      <c r="H8" s="12">
         <v>2573</v>
       </c>
-      <c r="H7" s="15">
+      <c r="I8" s="12">
         <v>443</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J8" s="4">
         <v>2507</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K8" s="4">
         <v>2353</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L8" s="5">
         <v>154</v>
       </c>
-      <c r="L7" s="15">
+      <c r="M8" s="12">
         <v>500</v>
       </c>
-      <c r="M7" s="25">
+      <c r="N8" s="20">
         <v>226</v>
       </c>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-    </row>
-    <row r="8" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="16">
+      <c r="C9" s="13">
         <v>509019</v>
       </c>
-      <c r="C8" s="15">
+      <c r="D9" s="12">
         <v>1034</v>
       </c>
-      <c r="D8" s="15">
+      <c r="E9" s="12">
         <v>623</v>
       </c>
-      <c r="E8" s="16">
+      <c r="F9" s="13">
         <v>3854</v>
       </c>
-      <c r="F8" s="15">
+      <c r="G9" s="12">
         <v>170</v>
       </c>
-      <c r="G8" s="15">
+      <c r="H9" s="12">
         <v>2502</v>
       </c>
-      <c r="H8" s="15">
+      <c r="I9" s="12">
         <v>460</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J9" s="4">
         <v>3276</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K9" s="4">
         <v>3136</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L9" s="5">
         <v>140</v>
       </c>
-      <c r="L8" s="15">
+      <c r="M9" s="12">
         <v>556</v>
       </c>
-      <c r="M8" s="25">
+      <c r="N9" s="20">
         <v>238</v>
       </c>
-      <c r="N8" s="32" t="s">
+      <c r="O9" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="32" t="s">
+      <c r="P9" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="P8" s="32" t="s">
+      <c r="Q9" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="32" t="s">
+      <c r="R9" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="36" t="s">
+      <c r="S9" s="29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+    <row r="10" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="16">
+      <c r="C10" s="13">
         <v>632547</v>
       </c>
-      <c r="C9" s="15">
+      <c r="D10" s="12">
         <v>1041</v>
       </c>
-      <c r="D9" s="15">
+      <c r="E10" s="12">
         <v>747</v>
       </c>
-      <c r="E9" s="16">
+      <c r="F10" s="13">
         <v>3212</v>
       </c>
-      <c r="F9" s="15">
+      <c r="G10" s="12">
         <v>123</v>
       </c>
-      <c r="G9" s="15">
+      <c r="H10" s="12">
         <v>2255</v>
       </c>
-      <c r="H9" s="15">
+      <c r="I10" s="12">
         <v>443</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J10" s="4">
         <v>3868</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K10" s="4">
         <v>3752</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L10" s="5">
         <v>116</v>
       </c>
-      <c r="L9" s="15">
+      <c r="M10" s="12">
         <v>580</v>
       </c>
-      <c r="M9" s="25">
+      <c r="N10" s="20">
         <v>259</v>
       </c>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-    </row>
-    <row r="10" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+    </row>
+    <row r="11" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="16">
+      <c r="C11" s="13">
         <v>519125</v>
       </c>
-      <c r="C10" s="15">
+      <c r="D11" s="12">
         <v>1050</v>
       </c>
-      <c r="D10" s="15">
+      <c r="E11" s="12">
         <v>696</v>
       </c>
-      <c r="E10" s="16">
+      <c r="F11" s="13">
         <v>3976</v>
       </c>
-      <c r="F10" s="15">
+      <c r="G11" s="12">
         <v>146</v>
       </c>
-      <c r="G10" s="15">
+      <c r="H11" s="12">
         <v>2424</v>
       </c>
-      <c r="H10" s="15">
+      <c r="I11" s="12">
         <v>476</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J11" s="4">
         <v>2889</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K11" s="4">
         <v>2721</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L11" s="5">
         <v>168</v>
       </c>
-      <c r="L10" s="15">
+      <c r="M11" s="12">
         <v>571</v>
       </c>
-      <c r="M10" s="25">
+      <c r="N11" s="20">
         <v>247</v>
       </c>
-      <c r="N10" s="30">
+      <c r="O11" s="23">
         <v>25.2</v>
       </c>
-      <c r="O10" s="30">
+      <c r="P11" s="23">
         <v>49.8</v>
       </c>
-      <c r="P10" s="30">
+      <c r="Q11" s="23">
         <v>20.5</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="R11" s="23">
         <v>7.5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+    <row r="12" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="16">
+      <c r="C12" s="13">
         <v>820580</v>
       </c>
-      <c r="C11" s="15">
+      <c r="D12" s="12">
         <v>1086</v>
       </c>
-      <c r="D11" s="15">
+      <c r="E12" s="12">
         <v>474</v>
       </c>
-      <c r="E11" s="16">
+      <c r="F12" s="13">
         <v>5466</v>
       </c>
-      <c r="F11" s="15">
+      <c r="G12" s="12">
         <v>157</v>
       </c>
-      <c r="G11" s="15">
+      <c r="H12" s="12">
         <v>2587</v>
       </c>
-      <c r="H11" s="15">
+      <c r="I12" s="12">
         <v>516</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J12" s="4">
         <v>3570</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K12" s="4">
         <v>3419</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L12" s="5">
         <v>151</v>
       </c>
-      <c r="L11" s="15">
+      <c r="M12" s="12">
         <v>523</v>
       </c>
-      <c r="M11" s="25">
+      <c r="N12" s="20">
         <v>277</v>
       </c>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-    </row>
-    <row r="12" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+    </row>
+    <row r="13" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="16">
+      <c r="C13" s="13">
         <v>295285</v>
       </c>
-      <c r="C12" s="15">
+      <c r="D13" s="12">
         <v>1122</v>
       </c>
-      <c r="D12" s="15">
+      <c r="E13" s="12">
         <v>460</v>
       </c>
-      <c r="E12" s="16">
+      <c r="F13" s="13">
         <v>3615</v>
       </c>
-      <c r="F12" s="15">
+      <c r="G13" s="12">
         <v>149</v>
       </c>
-      <c r="G12" s="15">
+      <c r="H13" s="12">
         <v>3015</v>
       </c>
-      <c r="H12" s="15">
+      <c r="I13" s="12">
         <v>584</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J13" s="4">
         <v>3134</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K13" s="4">
         <v>2968</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L13" s="5">
         <v>166</v>
       </c>
-      <c r="L12" s="15">
+      <c r="M13" s="12">
         <v>494</v>
       </c>
-      <c r="M12" s="25">
+      <c r="N13" s="20">
         <v>268</v>
       </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-    </row>
-    <row r="13" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="O13" s="22"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+    </row>
+    <row r="14" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="16">
+      <c r="C14" s="13">
         <v>441608</v>
       </c>
-      <c r="C13" s="15">
+      <c r="D14" s="12">
         <v>1159</v>
       </c>
-      <c r="D13" s="15">
+      <c r="E14" s="12">
         <v>543</v>
       </c>
-      <c r="E13" s="16">
+      <c r="F14" s="13">
         <v>5414</v>
       </c>
-      <c r="F13" s="15">
+      <c r="G14" s="12">
         <v>181</v>
       </c>
-      <c r="G13" s="15">
+      <c r="H14" s="12">
         <v>3228</v>
       </c>
-      <c r="H13" s="15">
+      <c r="I14" s="12">
         <v>590</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J14" s="4">
         <v>2338</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K14" s="4">
         <v>2142</v>
       </c>
-      <c r="K13" s="5">
+      <c r="L14" s="5">
         <v>196</v>
       </c>
-      <c r="L13" s="15">
+      <c r="M14" s="12">
         <v>533</v>
       </c>
-      <c r="M13" s="25">
+      <c r="N14" s="20">
         <v>287</v>
       </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-    </row>
-    <row r="14" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+    </row>
+    <row r="15" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="16">
+      <c r="C15" s="13">
         <v>582601</v>
       </c>
-      <c r="C14" s="15">
+      <c r="D15" s="12">
         <v>1269</v>
       </c>
-      <c r="D14" s="15">
+      <c r="E15" s="12">
         <v>587</v>
       </c>
-      <c r="E14" s="16">
+      <c r="F15" s="13">
         <v>5056</v>
       </c>
-      <c r="F14" s="15">
+      <c r="G15" s="12">
         <v>219</v>
       </c>
-      <c r="G14" s="15">
+      <c r="H15" s="12">
         <v>2716</v>
       </c>
-      <c r="H14" s="15">
+      <c r="I15" s="12">
         <v>527</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J15" s="4">
         <v>3371</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K15" s="4">
         <v>3255</v>
       </c>
-      <c r="K14" s="5">
+      <c r="L15" s="5">
         <v>116</v>
       </c>
-      <c r="L14" s="15">
+      <c r="M15" s="12">
         <v>538</v>
       </c>
-      <c r="M14" s="25">
+      <c r="N15" s="20">
         <v>260</v>
       </c>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-    </row>
-    <row r="15" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+    </row>
+    <row r="16" spans="1:19" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="16">
+      <c r="C16" s="13">
         <v>1360998</v>
       </c>
-      <c r="C15" s="15">
+      <c r="D16" s="12">
         <v>1311</v>
       </c>
-      <c r="D15" s="15">
+      <c r="E16" s="12">
         <v>732</v>
       </c>
-      <c r="E15" s="16">
+      <c r="F16" s="13">
         <v>4806</v>
       </c>
-      <c r="F15" s="15">
+      <c r="G16" s="12">
         <v>215</v>
       </c>
-      <c r="G15" s="15">
+      <c r="H16" s="12">
         <v>2577</v>
       </c>
-      <c r="H15" s="15">
+      <c r="I16" s="12">
         <v>577</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J16" s="4">
         <v>3613</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K16" s="4">
         <v>3414</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L16" s="5">
         <v>199</v>
       </c>
-      <c r="L15" s="15">
+      <c r="M16" s="12">
         <v>591</v>
       </c>
-      <c r="M15" s="25">
+      <c r="N16" s="20">
         <v>299</v>
       </c>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-    </row>
-    <row r="16" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+    </row>
+    <row r="17" spans="1:18" ht="33.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="16">
+      <c r="C17" s="13">
         <v>640909</v>
       </c>
-      <c r="C16" s="15">
+      <c r="D17" s="12">
         <v>1329</v>
       </c>
-      <c r="D16" s="15">
+      <c r="E17" s="12">
         <v>661</v>
       </c>
-      <c r="E16" s="15">
+      <c r="F17" s="12">
         <v>4918</v>
       </c>
-      <c r="F16" s="15">
+      <c r="G17" s="12">
         <v>196</v>
       </c>
-      <c r="G16" s="15">
+      <c r="H17" s="12">
         <v>2399</v>
       </c>
-      <c r="H16" s="15">
+      <c r="I17" s="12">
         <v>492</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J17" s="4">
         <v>3328</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K17" s="4">
         <v>3189</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L17" s="5">
         <v>139</v>
       </c>
-      <c r="L16" s="15">
+      <c r="M17" s="12">
         <v>557</v>
       </c>
-      <c r="M16" s="25">
+      <c r="N17" s="20">
         <v>254</v>
       </c>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-    </row>
-    <row r="17" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="29"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-    </row>
-    <row r="18" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+    </row>
+    <row r="18" spans="1:18" ht="33.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="23">
+      <c r="C18" s="18">
         <v>10626430</v>
       </c>
-      <c r="C18" s="19">
+      <c r="D18" s="14">
         <v>1106</v>
       </c>
-      <c r="D18" s="19">
+      <c r="E18" s="14">
         <v>612</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19">
+      <c r="F18" s="14"/>
+      <c r="G18" s="14">
         <v>164</v>
       </c>
-      <c r="G18" s="19">
+      <c r="H18" s="14">
         <v>2605</v>
       </c>
-      <c r="H18" s="19">
+      <c r="I18" s="14">
         <v>501</v>
       </c>
-      <c r="I18" s="9">
+      <c r="J18" s="6">
         <v>3325</v>
       </c>
-      <c r="J18" s="10">
+      <c r="K18" s="7">
         <v>3161</v>
       </c>
-      <c r="K18" s="11">
+      <c r="L18" s="8">
         <v>163</v>
       </c>
-      <c r="L18" s="19">
+      <c r="M18" s="14">
         <v>542</v>
       </c>
-      <c r="M18" s="20">
+      <c r="N18" s="15">
         <v>259</v>
       </c>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2">
+        <v>109</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3">
+        <v>181</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4">
+        <v>146</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5">
+        <v>137</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6">
+        <v>170</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7">
+        <v>123</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8">
+        <v>146</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9">
+        <v>157</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10">
+        <v>149</v>
+      </c>
+      <c r="I10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11">
+        <v>181</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12">
+        <v>219</v>
+      </c>
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13">
+        <v>215</v>
+      </c>
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14">
+        <v>196</v>
+      </c>
+      <c r="I14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>